<commit_message>
dodanie nowego pasa WAW
</commit_message>
<xml_diff>
--- a/Cesium/tablica_wspolrzednych.xlsx
+++ b/Cesium/tablica_wspolrzednych.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Lotnisko Gdansk</t>
   </si>
@@ -40,10 +40,22 @@
     <t>Koniec pasa #1</t>
   </si>
   <si>
-    <t>Roznica latitude</t>
-  </si>
-  <si>
-    <t>Roznica longitude</t>
+    <t>Poczatek pasa #2</t>
+  </si>
+  <si>
+    <t>Koniec pasa #2</t>
+  </si>
+  <si>
+    <t>Roznica latitude dla pas #1</t>
+  </si>
+  <si>
+    <t>Roznica longitude dla pas #1</t>
+  </si>
+  <si>
+    <t>Roznica latitude dla pas #2</t>
+  </si>
+  <si>
+    <t>Roznica longitude dla pas #2</t>
   </si>
 </sst>
 </file>
@@ -385,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,7 +438,7 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -443,17 +455,17 @@
         <v>18.489267000000002</v>
       </c>
       <c r="H4">
-        <f>D4-A10</f>
-        <v>2.2160030000000006</v>
+        <f>D4-D10</f>
+        <v>2.1947669999999988</v>
       </c>
       <c r="I4">
         <f>H4/5</f>
-        <v>0.44320060000000011</v>
+        <v>0.43895339999999977</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -461,12 +473,12 @@
         <v>5</v>
       </c>
       <c r="H7">
-        <f>B10-E4</f>
-        <v>2.486419999999999</v>
+        <f>E10-E4</f>
+        <v>2.4679099999999998</v>
       </c>
       <c r="I7">
         <f>H7/5</f>
-        <v>0.49728399999999978</v>
+        <v>0.49358199999999997</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -503,6 +515,68 @@
       </c>
       <c r="E10">
         <v>20.957177000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <f>D4-D15</f>
+        <v>2.201357999999999</v>
+      </c>
+      <c r="I14">
+        <f>H14/5</f>
+        <v>0.44027159999999982</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>52.162706</v>
+      </c>
+      <c r="B15">
+        <v>20.978023</v>
+      </c>
+      <c r="D15">
+        <v>52.170552000000001</v>
+      </c>
+      <c r="E15">
+        <v>20.950043999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H17">
+        <f>E15-E4</f>
+        <v>2.4607769999999967</v>
+      </c>
+      <c r="I17">
+        <f>H17/5</f>
+        <v>0.49215539999999935</v>
       </c>
     </row>
   </sheetData>

</xml_diff>